<commit_message>
Ejercicios con Listas enlazadas
</commit_message>
<xml_diff>
--- a/src/memoria/lista enlazada.xlsx
+++ b/src/memoria/lista enlazada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aula\Documents\NetBeansProjects\Programacion2_2_4_2016\src\memoria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aula\Documents\GitHub\Programacion2_2_4_2016\src\memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -232,30 +232,32 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>285747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>695326</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="14" name="Conector angular 13"/>
         <xdr:cNvCxnSpPr>
-          <a:endCxn id="2" idx="2"/>
+          <a:endCxn id="48" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1373981" y="1378743"/>
-          <a:ext cx="690563" cy="600075"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+          <a:off x="157162" y="2309811"/>
+          <a:ext cx="3133727" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -307,15 +309,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="accent4">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -347,26 +349,26 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>9</xdr:row>
       <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="18" name="Conector recto de flecha 17"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="17" idx="6"/>
-          <a:endCxn id="34" idx="2"/>
+          <a:endCxn id="30" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6124575" y="2033588"/>
-          <a:ext cx="876300" cy="9525"/>
+        <a:xfrm>
+          <a:off x="6124575" y="2043113"/>
+          <a:ext cx="133350" cy="1519237"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -394,16 +396,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>176346</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>320069</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -412,21 +414,23 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1800225" y="2986221"/>
-          <a:ext cx="805844" cy="1538154"/>
-          <a:chOff x="1590675" y="2881446"/>
-          <a:chExt cx="805844" cy="1538154"/>
+          <a:off x="4305300" y="2847975"/>
+          <a:ext cx="704850" cy="1066800"/>
+          <a:chOff x="1590675" y="3343275"/>
+          <a:chExt cx="704850" cy="1066800"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
           <xdr:cNvPr id="25" name="Conector recto de flecha 24"/>
-          <xdr:cNvCxnSpPr/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="26" idx="0"/>
+          </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipV="1">
-            <a:off x="1847850" y="2881446"/>
-            <a:ext cx="548669" cy="1300029"/>
+            <a:off x="1866900" y="3343275"/>
+            <a:ext cx="428625" cy="828675"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -457,7 +461,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1590675" y="4181475"/>
+            <a:off x="1590675" y="4171950"/>
             <a:ext cx="552450" cy="238125"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -505,15 +509,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -522,7 +526,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7000875" y="1009650"/>
+          <a:off x="7181850" y="1057275"/>
           <a:ext cx="1600200" cy="2047875"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -531,15 +535,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent4">
+          <a:schemeClr val="accent1">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent4"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -568,16 +572,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>746731</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>165706</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>138246</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>185871</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -589,8 +593,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8366731" y="2757621"/>
-          <a:ext cx="53369" cy="814254"/>
+          <a:off x="8547706" y="2805246"/>
+          <a:ext cx="815369" cy="757104"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -618,16 +622,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -636,7 +640,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620000" y="3571875"/>
+          <a:off x="8562975" y="3562350"/>
           <a:ext cx="1600200" cy="2047875"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -682,16 +686,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>185738</xdr:rowOff>
+      <xdr:rowOff>176213</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -702,8 +706,236 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9220200" y="4591050"/>
+          <a:off x="10163175" y="4581525"/>
           <a:ext cx="609600" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Elipse 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5400675" y="3562350"/>
+          <a:ext cx="1714500" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-HN" sz="2400"/>
+            <a:t>5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-HN" sz="2400"/>
+            <a:t>Frances</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Conector recto de flecha 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="30" idx="6"/>
+          <a:endCxn id="34" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7115175" y="3105150"/>
+          <a:ext cx="866775" cy="1481138"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Elipse 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1362075" y="4371975"/>
+          <a:ext cx="1714500" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-HN" sz="2400"/>
+            <a:t>6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-HN" sz="2400"/>
+            <a:t>Celeste</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Conector recto de flecha 48"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="48" idx="6"/>
+          <a:endCxn id="2" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2819400" y="3048000"/>
+          <a:ext cx="257175" cy="2347913"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -997,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>